<commit_message>
changed database colum, added gif file, corrected map logic
</commit_message>
<xml_diff>
--- a/excel-ona.xlsx
+++ b/excel-ona.xlsx
@@ -305,6 +305,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -386,18 +387,19 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D47"/>
+  <dimension ref="A1:E47"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A24" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F41" activeCellId="0" sqref="F41"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A26" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E39" activeCellId="0" sqref="E39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="2" min="1" style="0" width="18.7551020408163"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="18.1989795918367"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="55.2908163265306"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="23.7602040816327"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="55.2908163265306"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="11.5204081632653"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -410,9 +412,13 @@
       <c r="C1" s="0" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="0" t="str">
-        <f aca="false">"insert into county(c_code,county) values('"&amp;B1&amp;"','"&amp;C1&amp;"');"</f>
-        <v>insert into county(c_code,county) values('Keri','Kericho');</v>
+      <c r="D1" s="0" t="n">
+        <f aca="false">RANDBETWEEN(100,2000)</f>
+        <v>1354</v>
+      </c>
+      <c r="E1" s="0" t="str">
+        <f aca="false">"insert into county(c_code,county,value) values('"&amp;B1&amp;"','"&amp;C1&amp;"','"&amp;D1&amp;"');"</f>
+        <v>insert into county(c_code,county,value) values('Keri','Kericho','1354');</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -425,9 +431,13 @@
       <c r="C2" s="0" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="0" t="str">
-        <f aca="false">"insert into county(c_code,county) values('"&amp;B2&amp;"','"&amp;C2&amp;"');"</f>
-        <v>insert into county(c_code,county) values('Mand','Mandera');</v>
+      <c r="D2" s="0" t="n">
+        <f aca="false">RANDBETWEEN(100,2000)</f>
+        <v>1294</v>
+      </c>
+      <c r="E2" s="0" t="str">
+        <f aca="false">"insert into county(c_code,county,value) values('"&amp;B2&amp;"','"&amp;C2&amp;"','"&amp;D2&amp;"');"</f>
+        <v>insert into county(c_code,county,value) values('Mand','Mandera','1294');</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -440,9 +450,13 @@
       <c r="C3" s="0" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="0" t="str">
-        <f aca="false">"insert into county(c_code,county) values('"&amp;B3&amp;"','"&amp;C3&amp;"');"</f>
-        <v>insert into county(c_code,county) values('Waji','Wajir');</v>
+      <c r="D3" s="0" t="n">
+        <f aca="false">RANDBETWEEN(100,2000)</f>
+        <v>709</v>
+      </c>
+      <c r="E3" s="0" t="str">
+        <f aca="false">"insert into county(c_code,county,value) values('"&amp;B3&amp;"','"&amp;C3&amp;"','"&amp;D3&amp;"');"</f>
+        <v>insert into county(c_code,county,value) values('Waji','Wajir','709');</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -455,9 +469,13 @@
       <c r="C4" s="0" t="s">
         <v>7</v>
       </c>
-      <c r="D4" s="0" t="str">
-        <f aca="false">"insert into county(c_code,county) values('"&amp;B4&amp;"','"&amp;C4&amp;"');"</f>
-        <v>insert into county(c_code,county) values('Mars','Marsabit');</v>
+      <c r="D4" s="0" t="n">
+        <f aca="false">RANDBETWEEN(100,2000)</f>
+        <v>1048</v>
+      </c>
+      <c r="E4" s="0" t="str">
+        <f aca="false">"insert into county(c_code,county,value) values('"&amp;B4&amp;"','"&amp;C4&amp;"','"&amp;D4&amp;"');"</f>
+        <v>insert into county(c_code,county,value) values('Mars','Marsabit','1048');</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -470,9 +488,13 @@
       <c r="C5" s="0" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="0" t="str">
-        <f aca="false">"insert into county(c_code,county) values('"&amp;B5&amp;"','"&amp;C5&amp;"');"</f>
-        <v>insert into county(c_code,county) values('Isio','Isiolo');</v>
+      <c r="D5" s="0" t="n">
+        <f aca="false">RANDBETWEEN(100,2000)</f>
+        <v>193</v>
+      </c>
+      <c r="E5" s="0" t="str">
+        <f aca="false">"insert into county(c_code,county,value) values('"&amp;B5&amp;"','"&amp;C5&amp;"','"&amp;D5&amp;"');"</f>
+        <v>insert into county(c_code,county,value) values('Isio','Isiolo','193');</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -485,9 +507,13 @@
       <c r="C6" s="0" t="s">
         <v>11</v>
       </c>
-      <c r="D6" s="0" t="str">
-        <f aca="false">"insert into county(c_code,county) values('"&amp;B6&amp;"','"&amp;C6&amp;"');"</f>
-        <v>insert into county(c_code,county) values('Laik','Laikipia');</v>
+      <c r="D6" s="0" t="n">
+        <f aca="false">RANDBETWEEN(100,2000)</f>
+        <v>1053</v>
+      </c>
+      <c r="E6" s="0" t="str">
+        <f aca="false">"insert into county(c_code,county,value) values('"&amp;B6&amp;"','"&amp;C6&amp;"','"&amp;D6&amp;"');"</f>
+        <v>insert into county(c_code,county,value) values('Laik','Laikipia','1053');</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -500,9 +526,13 @@
       <c r="C7" s="0" t="s">
         <v>13</v>
       </c>
-      <c r="D7" s="0" t="str">
-        <f aca="false">"insert into county(c_code,county) values('"&amp;B7&amp;"','"&amp;C7&amp;"');"</f>
-        <v>insert into county(c_code,county) values('Gari','Garissa');</v>
+      <c r="D7" s="0" t="n">
+        <f aca="false">RANDBETWEEN(100,2000)</f>
+        <v>1429</v>
+      </c>
+      <c r="E7" s="0" t="str">
+        <f aca="false">"insert into county(c_code,county,value) values('"&amp;B7&amp;"','"&amp;C7&amp;"','"&amp;D7&amp;"');"</f>
+        <v>insert into county(c_code,county,value) values('Gari','Garissa','1429');</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -515,9 +545,13 @@
       <c r="C8" s="0" t="s">
         <v>14</v>
       </c>
-      <c r="D8" s="0" t="str">
-        <f aca="false">"insert into county(c_code,county) values('"&amp;B8&amp;"','"&amp;C8&amp;"');"</f>
-        <v>insert into county(c_code,county) values('Lamu','Lamu');</v>
+      <c r="D8" s="0" t="n">
+        <f aca="false">RANDBETWEEN(100,2000)</f>
+        <v>1404</v>
+      </c>
+      <c r="E8" s="0" t="str">
+        <f aca="false">"insert into county(c_code,county,value) values('"&amp;B8&amp;"','"&amp;C8&amp;"','"&amp;D8&amp;"');"</f>
+        <v>insert into county(c_code,county,value) values('Lamu','Lamu','1404');</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -530,9 +564,13 @@
       <c r="C9" s="0" t="s">
         <v>16</v>
       </c>
-      <c r="D9" s="0" t="str">
-        <f aca="false">"insert into county(c_code,county) values('"&amp;B9&amp;"','"&amp;C9&amp;"');"</f>
-        <v>insert into county(c_code,county) values('Tana','Tana River');</v>
+      <c r="D9" s="0" t="n">
+        <f aca="false">RANDBETWEEN(100,2000)</f>
+        <v>223</v>
+      </c>
+      <c r="E9" s="0" t="str">
+        <f aca="false">"insert into county(c_code,county,value) values('"&amp;B9&amp;"','"&amp;C9&amp;"','"&amp;D9&amp;"');"</f>
+        <v>insert into county(c_code,county,value) values('Tana','Tana River','223');</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -545,9 +583,13 @@
       <c r="C10" s="0" t="s">
         <v>18</v>
       </c>
-      <c r="D10" s="0" t="str">
-        <f aca="false">"insert into county(c_code,county) values('"&amp;B10&amp;"','"&amp;C10&amp;"');"</f>
-        <v>insert into county(c_code,county) values('Kili','Kilifi');</v>
+      <c r="D10" s="0" t="n">
+        <f aca="false">RANDBETWEEN(100,2000)</f>
+        <v>1596</v>
+      </c>
+      <c r="E10" s="0" t="str">
+        <f aca="false">"insert into county(c_code,county,value) values('"&amp;B10&amp;"','"&amp;C10&amp;"','"&amp;D10&amp;"');"</f>
+        <v>insert into county(c_code,county,value) values('Kili','Kilifi','1596');</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -560,9 +602,13 @@
       <c r="C11" s="0" t="s">
         <v>20</v>
       </c>
-      <c r="D11" s="0" t="str">
-        <f aca="false">"insert into county(c_code,county) values('"&amp;B11&amp;"','"&amp;C11&amp;"');"</f>
-        <v>insert into county(c_code,county) values('Kwal','Kwale');</v>
+      <c r="D11" s="0" t="n">
+        <f aca="false">RANDBETWEEN(100,2000)</f>
+        <v>1493</v>
+      </c>
+      <c r="E11" s="0" t="str">
+        <f aca="false">"insert into county(c_code,county,value) values('"&amp;B11&amp;"','"&amp;C11&amp;"','"&amp;D11&amp;"');"</f>
+        <v>insert into county(c_code,county,value) values('Kwal','Kwale','1493');</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -575,9 +621,13 @@
       <c r="C12" s="0" t="s">
         <v>22</v>
       </c>
-      <c r="D12" s="0" t="str">
-        <f aca="false">"insert into county(c_code,county) values('"&amp;B12&amp;"','"&amp;C12&amp;"');"</f>
-        <v>insert into county(c_code,county) values('Maku','Makueni');</v>
+      <c r="D12" s="0" t="n">
+        <f aca="false">RANDBETWEEN(100,2000)</f>
+        <v>1473</v>
+      </c>
+      <c r="E12" s="0" t="str">
+        <f aca="false">"insert into county(c_code,county,value) values('"&amp;B12&amp;"','"&amp;C12&amp;"','"&amp;D12&amp;"');"</f>
+        <v>insert into county(c_code,county,value) values('Maku','Makueni','1473');</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -590,9 +640,13 @@
       <c r="C13" s="0" t="s">
         <v>24</v>
       </c>
-      <c r="D13" s="0" t="str">
-        <f aca="false">"insert into county(c_code,county) values('"&amp;B13&amp;"','"&amp;C13&amp;"');"</f>
-        <v>insert into county(c_code,county) values('Tait','Taita Taveta');</v>
+      <c r="D13" s="0" t="n">
+        <f aca="false">RANDBETWEEN(100,2000)</f>
+        <v>1329</v>
+      </c>
+      <c r="E13" s="0" t="str">
+        <f aca="false">"insert into county(c_code,county,value) values('"&amp;B13&amp;"','"&amp;C13&amp;"','"&amp;D13&amp;"');"</f>
+        <v>insert into county(c_code,county,value) values('Tait','Taita Taveta','1329');</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -605,9 +659,13 @@
       <c r="C14" s="0" t="s">
         <v>26</v>
       </c>
-      <c r="D14" s="0" t="str">
-        <f aca="false">"insert into county(c_code,county) values('"&amp;B14&amp;"','"&amp;C14&amp;"');"</f>
-        <v>insert into county(c_code,county) values('Kitu','Kitui');</v>
+      <c r="D14" s="0" t="n">
+        <f aca="false">RANDBETWEEN(100,2000)</f>
+        <v>1316</v>
+      </c>
+      <c r="E14" s="0" t="str">
+        <f aca="false">"insert into county(c_code,county,value) values('"&amp;B14&amp;"','"&amp;C14&amp;"','"&amp;D14&amp;"');"</f>
+        <v>insert into county(c_code,county,value) values('Kitu','Kitui','1316');</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -620,9 +678,13 @@
       <c r="C15" s="0" t="s">
         <v>27</v>
       </c>
-      <c r="D15" s="0" t="str">
-        <f aca="false">"insert into county(c_code,county) values('"&amp;B15&amp;"','"&amp;C15&amp;"');"</f>
-        <v>insert into county(c_code,county) values('Meru','Meru');</v>
+      <c r="D15" s="0" t="n">
+        <f aca="false">RANDBETWEEN(100,2000)</f>
+        <v>786</v>
+      </c>
+      <c r="E15" s="0" t="str">
+        <f aca="false">"insert into county(c_code,county,value) values('"&amp;B15&amp;"','"&amp;C15&amp;"','"&amp;D15&amp;"');"</f>
+        <v>insert into county(c_code,county,value) values('Meru','Meru','786');</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -635,9 +697,13 @@
       <c r="C16" s="0" t="s">
         <v>29</v>
       </c>
-      <c r="D16" s="0" t="str">
-        <f aca="false">"insert into county(c_code,county) values('"&amp;B16&amp;"','"&amp;C16&amp;"');"</f>
-        <v>insert into county(c_code,county) values('Nyer','Nyeri');</v>
+      <c r="D16" s="0" t="n">
+        <f aca="false">RANDBETWEEN(100,2000)</f>
+        <v>128</v>
+      </c>
+      <c r="E16" s="0" t="str">
+        <f aca="false">"insert into county(c_code,county,value) values('"&amp;B16&amp;"','"&amp;C16&amp;"','"&amp;D16&amp;"');"</f>
+        <v>insert into county(c_code,county,value) values('Nyer','Nyeri','128');</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -650,9 +716,13 @@
       <c r="C17" s="0" t="s">
         <v>31</v>
       </c>
-      <c r="D17" s="0" t="str">
-        <f aca="false">"insert into county(c_code,county) values('"&amp;B17&amp;"','"&amp;C17&amp;"');"</f>
-        <v>insert into county(c_code,county) values('Emb','Embu');</v>
+      <c r="D17" s="0" t="n">
+        <f aca="false">RANDBETWEEN(100,2000)</f>
+        <v>1172</v>
+      </c>
+      <c r="E17" s="0" t="str">
+        <f aca="false">"insert into county(c_code,county,value) values('"&amp;B17&amp;"','"&amp;C17&amp;"','"&amp;D17&amp;"');"</f>
+        <v>insert into county(c_code,county,value) values('Emb','Embu','1172');</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -665,9 +735,13 @@
       <c r="C18" s="0" t="s">
         <v>33</v>
       </c>
-      <c r="D18" s="0" t="str">
-        <f aca="false">"insert into county(c_code,county) values('"&amp;B18&amp;"','"&amp;C18&amp;"');"</f>
-        <v>insert into county(c_code,county) values('Thar','Tharaka Nithi');</v>
+      <c r="D18" s="0" t="n">
+        <f aca="false">RANDBETWEEN(100,2000)</f>
+        <v>246</v>
+      </c>
+      <c r="E18" s="0" t="str">
+        <f aca="false">"insert into county(c_code,county,value) values('"&amp;B18&amp;"','"&amp;C18&amp;"','"&amp;D18&amp;"');"</f>
+        <v>insert into county(c_code,county,value) values('Thar','Tharaka Nithi','246');</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -680,9 +754,13 @@
       <c r="C19" s="0" t="s">
         <v>35</v>
       </c>
-      <c r="D19" s="0" t="str">
-        <f aca="false">"insert into county(c_code,county) values('"&amp;B19&amp;"','"&amp;C19&amp;"');"</f>
-        <v>insert into county(c_code,county) values('Mach','Machakos');</v>
+      <c r="D19" s="0" t="n">
+        <f aca="false">RANDBETWEEN(100,2000)</f>
+        <v>128</v>
+      </c>
+      <c r="E19" s="0" t="str">
+        <f aca="false">"insert into county(c_code,county,value) values('"&amp;B19&amp;"','"&amp;C19&amp;"','"&amp;D19&amp;"');"</f>
+        <v>insert into county(c_code,county,value) values('Mach','Machakos','128');</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -695,9 +773,13 @@
       <c r="C20" s="0" t="s">
         <v>37</v>
       </c>
-      <c r="D20" s="0" t="str">
-        <f aca="false">"insert into county(c_code,county) values('"&amp;B20&amp;"','"&amp;C20&amp;"');"</f>
-        <v>insert into county(c_code,county) values('Kaji','Kajiado');</v>
+      <c r="D20" s="0" t="n">
+        <f aca="false">RANDBETWEEN(100,2000)</f>
+        <v>1930</v>
+      </c>
+      <c r="E20" s="0" t="str">
+        <f aca="false">"insert into county(c_code,county,value) values('"&amp;B20&amp;"','"&amp;C20&amp;"','"&amp;D20&amp;"');"</f>
+        <v>insert into county(c_code,county,value) values('Kaji','Kajiado','1930');</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -710,9 +792,13 @@
       <c r="C21" s="0" t="s">
         <v>39</v>
       </c>
-      <c r="D21" s="0" t="str">
-        <f aca="false">"insert into county(c_code,county) values('"&amp;B21&amp;"','"&amp;C21&amp;"');"</f>
-        <v>insert into county(c_code,county) values('Naro','Narok');</v>
+      <c r="D21" s="0" t="n">
+        <f aca="false">RANDBETWEEN(100,2000)</f>
+        <v>672</v>
+      </c>
+      <c r="E21" s="0" t="str">
+        <f aca="false">"insert into county(c_code,county,value) values('"&amp;B21&amp;"','"&amp;C21&amp;"','"&amp;D21&amp;"');"</f>
+        <v>insert into county(c_code,county,value) values('Naro','Narok','672');</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -725,9 +811,13 @@
       <c r="C22" s="0" t="s">
         <v>41</v>
       </c>
-      <c r="D22" s="0" t="str">
-        <f aca="false">"insert into county(c_code,county) values('"&amp;B22&amp;"','"&amp;C22&amp;"');"</f>
-        <v>insert into county(c_code,county) values('Migo','Migori');</v>
+      <c r="D22" s="0" t="n">
+        <f aca="false">RANDBETWEEN(100,2000)</f>
+        <v>742</v>
+      </c>
+      <c r="E22" s="0" t="str">
+        <f aca="false">"insert into county(c_code,county,value) values('"&amp;B22&amp;"','"&amp;C22&amp;"','"&amp;D22&amp;"');"</f>
+        <v>insert into county(c_code,county,value) values('Migo','Migori','742');</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -740,9 +830,13 @@
       <c r="C23" s="0" t="s">
         <v>43</v>
       </c>
-      <c r="D23" s="0" t="str">
-        <f aca="false">"insert into county(c_code,county) values('"&amp;B23&amp;"','"&amp;C23&amp;"');"</f>
-        <v>insert into county(c_code,county) values('Naku','Nakuru');</v>
+      <c r="D23" s="0" t="n">
+        <f aca="false">RANDBETWEEN(100,2000)</f>
+        <v>908</v>
+      </c>
+      <c r="E23" s="0" t="str">
+        <f aca="false">"insert into county(c_code,county,value) values('"&amp;B23&amp;"','"&amp;C23&amp;"','"&amp;D23&amp;"');"</f>
+        <v>insert into county(c_code,county,value) values('Naku','Nakuru','908');</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -755,9 +849,13 @@
       <c r="C24" s="0" t="s">
         <v>45</v>
       </c>
-      <c r="D24" s="0" t="str">
-        <f aca="false">"insert into county(c_code,county) values('"&amp;B24&amp;"','"&amp;C24&amp;"');"</f>
-        <v>insert into county(c_code,county) values('Bome','Bomet');</v>
+      <c r="D24" s="0" t="n">
+        <f aca="false">RANDBETWEEN(100,2000)</f>
+        <v>222</v>
+      </c>
+      <c r="E24" s="0" t="str">
+        <f aca="false">"insert into county(c_code,county,value) values('"&amp;B24&amp;"','"&amp;C24&amp;"','"&amp;D24&amp;"');"</f>
+        <v>insert into county(c_code,county,value) values('Bome','Bomet','222');</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -770,9 +868,13 @@
       <c r="C25" s="0" t="s">
         <v>47</v>
       </c>
-      <c r="D25" s="0" t="str">
-        <f aca="false">"insert into county(c_code,county) values('"&amp;B25&amp;"','"&amp;C25&amp;"');"</f>
-        <v>insert into county(c_code,county) values('Bari','Baringo');</v>
+      <c r="D25" s="0" t="n">
+        <f aca="false">RANDBETWEEN(100,2000)</f>
+        <v>1988</v>
+      </c>
+      <c r="E25" s="0" t="str">
+        <f aca="false">"insert into county(c_code,county,value) values('"&amp;B25&amp;"','"&amp;C25&amp;"','"&amp;D25&amp;"');"</f>
+        <v>insert into county(c_code,county,value) values('Bari','Baringo','1988');</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -785,9 +887,13 @@
       <c r="C26" s="0" t="s">
         <v>49</v>
       </c>
-      <c r="D26" s="0" t="str">
-        <f aca="false">"insert into county(c_code,county) values('"&amp;B26&amp;"','"&amp;C26&amp;"');"</f>
-        <v>insert into county(c_code,county) values('Turk','Turkana');</v>
+      <c r="D26" s="0" t="n">
+        <f aca="false">RANDBETWEEN(100,2000)</f>
+        <v>278</v>
+      </c>
+      <c r="E26" s="0" t="str">
+        <f aca="false">"insert into county(c_code,county,value) values('"&amp;B26&amp;"','"&amp;C26&amp;"','"&amp;D26&amp;"');"</f>
+        <v>insert into county(c_code,county,value) values('Turk','Turkana','278');</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -800,9 +906,13 @@
       <c r="C27" s="0" t="s">
         <v>51</v>
       </c>
-      <c r="D27" s="0" t="str">
-        <f aca="false">"insert into county(c_code,county) values('"&amp;B27&amp;"','"&amp;C27&amp;"');"</f>
-        <v>insert into county(c_code,county) values('West','West Pokot');</v>
+      <c r="D27" s="0" t="n">
+        <f aca="false">RANDBETWEEN(100,2000)</f>
+        <v>137</v>
+      </c>
+      <c r="E27" s="0" t="str">
+        <f aca="false">"insert into county(c_code,county,value) values('"&amp;B27&amp;"','"&amp;C27&amp;"','"&amp;D27&amp;"');"</f>
+        <v>insert into county(c_code,county,value) values('West','West Pokot','137');</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -815,9 +925,13 @@
       <c r="C28" s="0" t="s">
         <v>53</v>
       </c>
-      <c r="D28" s="0" t="str">
-        <f aca="false">"insert into county(c_code,county) values('"&amp;B28&amp;"','"&amp;C28&amp;"');"</f>
-        <v>insert into county(c_code,county) values('Samb','Samburu');</v>
+      <c r="D28" s="0" t="n">
+        <f aca="false">RANDBETWEEN(100,2000)</f>
+        <v>689</v>
+      </c>
+      <c r="E28" s="0" t="str">
+        <f aca="false">"insert into county(c_code,county,value) values('"&amp;B28&amp;"','"&amp;C28&amp;"','"&amp;D28&amp;"');"</f>
+        <v>insert into county(c_code,county,value) values('Samb','Samburu','689');</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -830,9 +944,13 @@
       <c r="C29" s="0" t="s">
         <v>55</v>
       </c>
-      <c r="D29" s="0" t="str">
-        <f aca="false">"insert into county(c_code,county) values('"&amp;B29&amp;"','"&amp;C29&amp;"');"</f>
-        <v>insert into county(c_code,county) values('Tran','Trans Nzoia');</v>
+      <c r="D29" s="0" t="n">
+        <f aca="false">RANDBETWEEN(100,2000)</f>
+        <v>883</v>
+      </c>
+      <c r="E29" s="0" t="str">
+        <f aca="false">"insert into county(c_code,county,value) values('"&amp;B29&amp;"','"&amp;C29&amp;"','"&amp;D29&amp;"');"</f>
+        <v>insert into county(c_code,county,value) values('Tran','Trans Nzoia','883');</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -845,9 +963,13 @@
       <c r="C30" s="0" t="s">
         <v>57</v>
       </c>
-      <c r="D30" s="0" t="str">
-        <f aca="false">"insert into county(c_code,county) values('"&amp;B30&amp;"','"&amp;C30&amp;"');"</f>
-        <v>insert into county(c_code,county) values('Bung','Bungoma');</v>
+      <c r="D30" s="0" t="n">
+        <f aca="false">RANDBETWEEN(100,2000)</f>
+        <v>163</v>
+      </c>
+      <c r="E30" s="0" t="str">
+        <f aca="false">"insert into county(c_code,county,value) values('"&amp;B30&amp;"','"&amp;C30&amp;"','"&amp;D30&amp;"');"</f>
+        <v>insert into county(c_code,county,value) values('Bung','Bungoma','163');</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -860,9 +982,13 @@
       <c r="C31" s="0" t="s">
         <v>59</v>
       </c>
-      <c r="D31" s="0" t="str">
-        <f aca="false">"insert into county(c_code,county) values('"&amp;B31&amp;"','"&amp;C31&amp;"');"</f>
-        <v>insert into county(c_code,county) values('Uasi','Uasin Gishu');</v>
+      <c r="D31" s="0" t="n">
+        <f aca="false">RANDBETWEEN(100,2000)</f>
+        <v>495</v>
+      </c>
+      <c r="E31" s="0" t="str">
+        <f aca="false">"insert into county(c_code,county,value) values('"&amp;B31&amp;"','"&amp;C31&amp;"','"&amp;D31&amp;"');"</f>
+        <v>insert into county(c_code,county,value) values('Uasi','Uasin Gishu','495');</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -875,9 +1001,13 @@
       <c r="C32" s="0" t="s">
         <v>61</v>
       </c>
-      <c r="D32" s="0" t="str">
-        <f aca="false">"insert into county(c_code,county) values('"&amp;B32&amp;"','"&amp;C32&amp;"');"</f>
-        <v>insert into county(c_code,county) values('Busi','Busia');</v>
+      <c r="D32" s="0" t="n">
+        <f aca="false">RANDBETWEEN(100,2000)</f>
+        <v>237</v>
+      </c>
+      <c r="E32" s="0" t="str">
+        <f aca="false">"insert into county(c_code,county,value) values('"&amp;B32&amp;"','"&amp;C32&amp;"','"&amp;D32&amp;"');"</f>
+        <v>insert into county(c_code,county,value) values('Busi','Busia','237');</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -890,9 +1020,13 @@
       <c r="C33" s="0" t="s">
         <v>63</v>
       </c>
-      <c r="D33" s="0" t="str">
-        <f aca="false">"insert into county(c_code,county) values('"&amp;B33&amp;"','"&amp;C33&amp;"');"</f>
-        <v>insert into county(c_code,county) values('Kaka','Kakamega');</v>
+      <c r="D33" s="0" t="n">
+        <f aca="false">RANDBETWEEN(100,2000)</f>
+        <v>1358</v>
+      </c>
+      <c r="E33" s="0" t="str">
+        <f aca="false">"insert into county(c_code,county,value) values('"&amp;B33&amp;"','"&amp;C33&amp;"','"&amp;D33&amp;"');"</f>
+        <v>insert into county(c_code,county,value) values('Kaka','Kakamega','1358');</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -905,9 +1039,13 @@
       <c r="C34" s="0" t="s">
         <v>65</v>
       </c>
-      <c r="D34" s="0" t="str">
-        <f aca="false">"insert into county(c_code,county) values('"&amp;B34&amp;"','"&amp;C34&amp;"');"</f>
-        <v>insert into county(c_code,county) values('Siay','Siaya');</v>
+      <c r="D34" s="0" t="n">
+        <f aca="false">RANDBETWEEN(100,2000)</f>
+        <v>1104</v>
+      </c>
+      <c r="E34" s="0" t="str">
+        <f aca="false">"insert into county(c_code,county,value) values('"&amp;B34&amp;"','"&amp;C34&amp;"','"&amp;D34&amp;"');"</f>
+        <v>insert into county(c_code,county,value) values('Siay','Siaya','1104');</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -920,9 +1058,13 @@
       <c r="C35" s="0" t="s">
         <v>67</v>
       </c>
-      <c r="D35" s="0" t="str">
-        <f aca="false">"insert into county(c_code,county) values('"&amp;B35&amp;"','"&amp;C35&amp;"');"</f>
-        <v>insert into county(c_code,county) values('Homa','Homa Bay');</v>
+      <c r="D35" s="0" t="n">
+        <f aca="false">RANDBETWEEN(100,2000)</f>
+        <v>1186</v>
+      </c>
+      <c r="E35" s="0" t="str">
+        <f aca="false">"insert into county(c_code,county,value) values('"&amp;B35&amp;"','"&amp;C35&amp;"','"&amp;D35&amp;"');"</f>
+        <v>insert into county(c_code,county,value) values('Homa','Homa Bay','1186');</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -935,9 +1077,13 @@
       <c r="C36" s="0" t="s">
         <v>69</v>
       </c>
-      <c r="D36" s="0" t="str">
-        <f aca="false">"insert into county(c_code,county) values('"&amp;B36&amp;"','"&amp;C36&amp;"');"</f>
-        <v>insert into county(c_code,county) values('Kisu','Kisumu');</v>
+      <c r="D36" s="0" t="n">
+        <f aca="false">RANDBETWEEN(100,2000)</f>
+        <v>1451</v>
+      </c>
+      <c r="E36" s="0" t="str">
+        <f aca="false">"insert into county(c_code,county,value) values('"&amp;B36&amp;"','"&amp;C36&amp;"','"&amp;D36&amp;"');"</f>
+        <v>insert into county(c_code,county,value) values('Kisu','Kisumu','1451');</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -950,9 +1096,13 @@
       <c r="C37" s="0" t="s">
         <v>71</v>
       </c>
-      <c r="D37" s="0" t="str">
-        <f aca="false">"insert into county(c_code,county) values('"&amp;B37&amp;"','"&amp;C37&amp;"');"</f>
-        <v>insert into county(c_code,county) values('Vihi','Vihiga');</v>
+      <c r="D37" s="0" t="n">
+        <f aca="false">RANDBETWEEN(100,2000)</f>
+        <v>156</v>
+      </c>
+      <c r="E37" s="0" t="str">
+        <f aca="false">"insert into county(c_code,county,value) values('"&amp;B37&amp;"','"&amp;C37&amp;"','"&amp;D37&amp;"');"</f>
+        <v>insert into county(c_code,county,value) values('Vihi','Vihiga','156');</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -965,9 +1115,13 @@
       <c r="C38" s="0" t="s">
         <v>73</v>
       </c>
-      <c r="D38" s="0" t="str">
-        <f aca="false">"insert into county(c_code,county) values('"&amp;B38&amp;"','"&amp;C38&amp;"');"</f>
-        <v>insert into county(c_code,county) values('Nand','Nandi');</v>
+      <c r="D38" s="0" t="n">
+        <f aca="false">RANDBETWEEN(100,2000)</f>
+        <v>615</v>
+      </c>
+      <c r="E38" s="0" t="str">
+        <f aca="false">"insert into county(c_code,county,value) values('"&amp;B38&amp;"','"&amp;C38&amp;"','"&amp;D38&amp;"');"</f>
+        <v>insert into county(c_code,county,value) values('Nand','Nandi','615');</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -980,9 +1134,13 @@
       <c r="C39" s="0" t="s">
         <v>75</v>
       </c>
-      <c r="D39" s="0" t="str">
-        <f aca="false">"insert into county(c_code,county) values('"&amp;B39&amp;"','"&amp;C39&amp;"');"</f>
-        <v>insert into county(c_code,county) values('Elge','Elgeyo Marakwet');</v>
+      <c r="D39" s="0" t="n">
+        <f aca="false">RANDBETWEEN(100,2000)</f>
+        <v>855</v>
+      </c>
+      <c r="E39" s="0" t="str">
+        <f aca="false">"insert into county(c_code,county,value) values('"&amp;B39&amp;"','"&amp;C39&amp;"','"&amp;D39&amp;"');"</f>
+        <v>insert into county(c_code,county,value) values('Elge','Elgeyo Marakwet','855');</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -995,9 +1153,13 @@
       <c r="C40" s="0" t="s">
         <v>77</v>
       </c>
-      <c r="D40" s="0" t="str">
-        <f aca="false">"insert into county(c_code,county) values('"&amp;B40&amp;"','"&amp;C40&amp;"');"</f>
-        <v>insert into county(c_code,county) values('Nyam','Nyamira');</v>
+      <c r="D40" s="0" t="n">
+        <f aca="false">RANDBETWEEN(100,2000)</f>
+        <v>279</v>
+      </c>
+      <c r="E40" s="0" t="str">
+        <f aca="false">"insert into county(c_code,county,value) values('"&amp;B40&amp;"','"&amp;C40&amp;"','"&amp;D40&amp;"');"</f>
+        <v>insert into county(c_code,county,value) values('Nyam','Nyamira','279');</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1010,9 +1172,13 @@
       <c r="C41" s="0" t="s">
         <v>79</v>
       </c>
-      <c r="D41" s="0" t="str">
-        <f aca="false">"insert into county(c_code,county) values('"&amp;B41&amp;"','"&amp;C41&amp;"');"</f>
-        <v>insert into county(c_code,county) values('Kisi','Kisii');</v>
+      <c r="D41" s="0" t="n">
+        <f aca="false">RANDBETWEEN(100,2000)</f>
+        <v>210</v>
+      </c>
+      <c r="E41" s="0" t="str">
+        <f aca="false">"insert into county(c_code,county,value) values('"&amp;B41&amp;"','"&amp;C41&amp;"','"&amp;D41&amp;"');"</f>
+        <v>insert into county(c_code,county,value) values('Kisi','Kisii','210');</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1025,9 +1191,13 @@
       <c r="C42" s="0" t="s">
         <v>81</v>
       </c>
-      <c r="D42" s="0" t="str">
-        <f aca="false">"insert into county(c_code,county) values('"&amp;B42&amp;"','"&amp;C42&amp;"');"</f>
-        <v>insert into county(c_code,county) values('Mura','Muranga');</v>
+      <c r="D42" s="0" t="n">
+        <f aca="false">RANDBETWEEN(100,2000)</f>
+        <v>347</v>
+      </c>
+      <c r="E42" s="0" t="str">
+        <f aca="false">"insert into county(c_code,county,value) values('"&amp;B42&amp;"','"&amp;C42&amp;"','"&amp;D42&amp;"');"</f>
+        <v>insert into county(c_code,county,value) values('Mura','Muranga','347');</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1040,9 +1210,13 @@
       <c r="C43" s="0" t="s">
         <v>83</v>
       </c>
-      <c r="D43" s="0" t="str">
-        <f aca="false">"insert into county(c_code,county) values('"&amp;B43&amp;"','"&amp;C43&amp;"');"</f>
-        <v>insert into county(c_code,county) values('Kiri','Kirinyaga');</v>
+      <c r="D43" s="0" t="n">
+        <f aca="false">RANDBETWEEN(100,2000)</f>
+        <v>1653</v>
+      </c>
+      <c r="E43" s="0" t="str">
+        <f aca="false">"insert into county(c_code,county,value) values('"&amp;B43&amp;"','"&amp;C43&amp;"','"&amp;D43&amp;"');"</f>
+        <v>insert into county(c_code,county,value) values('Kiri','Kirinyaga','1653');</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1055,9 +1229,13 @@
       <c r="C44" s="0" t="s">
         <v>85</v>
       </c>
-      <c r="D44" s="0" t="str">
-        <f aca="false">"insert into county(c_code,county) values('"&amp;B44&amp;"','"&amp;C44&amp;"');"</f>
-        <v>insert into county(c_code,county) values('Kiam','Kiambu');</v>
+      <c r="D44" s="0" t="n">
+        <f aca="false">RANDBETWEEN(100,2000)</f>
+        <v>1439</v>
+      </c>
+      <c r="E44" s="0" t="str">
+        <f aca="false">"insert into county(c_code,county,value) values('"&amp;B44&amp;"','"&amp;C44&amp;"','"&amp;D44&amp;"');"</f>
+        <v>insert into county(c_code,county,value) values('Kiam','Kiambu','1439');</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1070,9 +1248,13 @@
       <c r="C45" s="0" t="s">
         <v>87</v>
       </c>
-      <c r="D45" s="0" t="str">
-        <f aca="false">"insert into county(c_code,county) values('"&amp;B45&amp;"','"&amp;C45&amp;"');"</f>
-        <v>insert into county(c_code,county) values('Nair','Nairobi');</v>
+      <c r="D45" s="0" t="n">
+        <f aca="false">RANDBETWEEN(100,2000)</f>
+        <v>1564</v>
+      </c>
+      <c r="E45" s="0" t="str">
+        <f aca="false">"insert into county(c_code,county,value) values('"&amp;B45&amp;"','"&amp;C45&amp;"','"&amp;D45&amp;"');"</f>
+        <v>insert into county(c_code,county,value) values('Nair','Nairobi','1564');</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1085,9 +1267,13 @@
       <c r="C46" s="0" t="s">
         <v>89</v>
       </c>
-      <c r="D46" s="0" t="str">
-        <f aca="false">"insert into county(c_code,county) values('"&amp;B46&amp;"','"&amp;C46&amp;"');"</f>
-        <v>insert into county(c_code,county) values('Nyan','Nyandarua');</v>
+      <c r="D46" s="0" t="n">
+        <f aca="false">RANDBETWEEN(100,2000)</f>
+        <v>438</v>
+      </c>
+      <c r="E46" s="0" t="str">
+        <f aca="false">"insert into county(c_code,county,value) values('"&amp;B46&amp;"','"&amp;C46&amp;"','"&amp;D46&amp;"');"</f>
+        <v>insert into county(c_code,county,value) values('Nyan','Nyandarua','438');</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1100,9 +1286,13 @@
       <c r="C47" s="0" t="s">
         <v>91</v>
       </c>
-      <c r="D47" s="0" t="str">
-        <f aca="false">"insert into county(c_code,county) values('"&amp;B47&amp;"','"&amp;C47&amp;"');"</f>
-        <v>insert into county(c_code,county) values('Momb','Mombasa');</v>
+      <c r="D47" s="0" t="n">
+        <f aca="false">RANDBETWEEN(100,2000)</f>
+        <v>1468</v>
+      </c>
+      <c r="E47" s="0" t="str">
+        <f aca="false">"insert into county(c_code,county,value) values('"&amp;B47&amp;"','"&amp;C47&amp;"','"&amp;D47&amp;"');"</f>
+        <v>insert into county(c_code,county,value) values('Momb','Mombasa','1468');</v>
       </c>
     </row>
   </sheetData>

</xml_diff>